<commit_message>
Country and Continent Data excel
</commit_message>
<xml_diff>
--- a/data/clean_data/CountryandContinentsData-excel.xlsx
+++ b/data/clean_data/CountryandContinentsData-excel.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\homework\FinalProject\Final_Team_Project\data\clean_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF185DC9-42C7-4655-8460-6F25CC0793D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB22AA3-6715-42FB-B7E8-97883A82E12F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="0" windowWidth="14430" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CountryandContinentsData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="553">
   <si>
     <t>Country</t>
   </si>
@@ -1625,6 +1636,60 @@
   </si>
   <si>
     <t>Taiwan</t>
+  </si>
+  <si>
+    <t>China Hong Kong SAR</t>
+  </si>
+  <si>
+    <t>Other Asia Pacific</t>
+  </si>
+  <si>
+    <t>Other Caribbean</t>
+  </si>
+  <si>
+    <t>Other CIS</t>
+  </si>
+  <si>
+    <t>Other Europe</t>
+  </si>
+  <si>
+    <t>Other Middle East</t>
+  </si>
+  <si>
+    <t>Other Northern Africa</t>
+  </si>
+  <si>
+    <t>Other South America</t>
+  </si>
+  <si>
+    <t>Other Southern Africa</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>Total Africa</t>
+  </si>
+  <si>
+    <t>Total Asia Pacific</t>
+  </si>
+  <si>
+    <t>Total CIS</t>
+  </si>
+  <si>
+    <t>Total Europe</t>
+  </si>
+  <si>
+    <t>Total Middle East</t>
+  </si>
+  <si>
+    <t>Total North America</t>
+  </si>
+  <si>
+    <t>Total S. &amp; Cent. America</t>
+  </si>
+  <si>
+    <t>Total World</t>
   </si>
 </sst>
 </file>
@@ -1767,7 +1832,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1947,6 +2012,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -2108,9 +2179,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2468,13 +2540,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E253"/>
+  <dimension ref="A1:E275"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -6331,6 +6406,182 @@
       </c>
       <c r="E253" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E254" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="E255" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E256" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E257" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="E258" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="E259" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="E260" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="E261" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="E262" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="E263" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="E264" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="E265" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="E266" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="E267" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E268" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A269" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="E269" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A270" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E270" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="E271" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A272" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E272" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="E273" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="E274" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A275" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E275" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>